<commit_message>
Removed the other sheets
</commit_message>
<xml_diff>
--- a/public/docs/EDARP_samples_being_referred_to _KNH_CCC_laboratory.xlsx
+++ b/public/docs/EDARP_samples_being_referred_to _KNH_CCC_laboratory.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bakasa\code\lab\public\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA01716-83C5-4463-8F3A-2DB68EE34A33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -150,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -795,6 +799,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -842,7 +849,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -875,9 +882,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -910,6 +934,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1085,7 +1126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z502"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A430" workbookViewId="0">
@@ -34864,28 +34905,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>